<commit_message>
change path to relative path 28/7/2022
</commit_message>
<xml_diff>
--- a/Connect/TestCase/020-reorder-submission/Default.xlsx
+++ b/Connect/TestCase/020-reorder-submission/Default.xlsx
@@ -239,10 +239,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="283845"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>

</xml_diff>